<commit_message>
push from d for c
</commit_message>
<xml_diff>
--- a/TelcobrightVS13/Projects/UtilInstallConfig/config/cas/_helper/casOperatorInfo.xlsx
+++ b/TelcobrightVS13/Projects/UtilInstallConfig/config/cas/_helper/casOperatorInfo.xlsx
@@ -2423,7 +2423,7 @@
     <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="L19" sqref="L19"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -2556,7 +2556,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="22" t="s">
         <v>4</v>
@@ -2647,7 +2647,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="22" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Huge changes from .5
</commit_message>
<xml_diff>
--- a/TelcobrightVS13/Projects/UtilInstallConfig/config/cas/_helper/casOperatorInfo.xlsx
+++ b/TelcobrightVS13/Projects/UtilInstallConfig/config/cas/_helper/casOperatorInfo.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="352">
   <si>
     <t>operator</t>
   </si>
@@ -626,7 +626,13 @@
     <t>j:\telcobright\vault\resources\cdr\mothertelecom\ip</t>
   </si>
   <si>
-    <t>vaultDialogic</t>
+    <t>C_sdr</t>
+  </si>
+  <si>
+    <t>.csv</t>
+  </si>
+  <si>
+    <t>vault.Dialogic</t>
   </si>
   <si>
     <t>10.154.150.55</t>
@@ -1056,9 +1062,6 @@
   </si>
   <si>
     <t>cdr</t>
-  </si>
-  <si>
-    <t>.csv</t>
   </si>
   <si>
     <t>CF</t>
@@ -2420,10 +2423,10 @@
   <sheetPr/>
   <dimension ref="A1:AD55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="72" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="72" topLeftCell="T1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="W54" sqref="W54"/>
+      <selection pane="bottomLeft" activeCell="AG49" sqref="AG49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -2593,10 +2596,10 @@
         <v>36</v>
       </c>
       <c r="O2" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q2" s="23">
         <v>1</v>
@@ -2621,7 +2624,7 @@
       </c>
       <c r="X2" s="22"/>
       <c r="Y2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z2">
         <v>1</v>
@@ -2686,10 +2689,10 @@
         <v>44</v>
       </c>
       <c r="O3" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3" s="23">
         <v>1</v>
@@ -2778,10 +2781,10 @@
         <v>36</v>
       </c>
       <c r="O4" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="23">
         <v>1</v>
@@ -2806,7 +2809,7 @@
       </c>
       <c r="X4" s="22"/>
       <c r="Y4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z4">
         <v>1</v>
@@ -2866,10 +2869,10 @@
         <v>36</v>
       </c>
       <c r="O5" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5" s="23">
         <v>1</v>
@@ -2894,7 +2897,7 @@
       </c>
       <c r="X5" s="22"/>
       <c r="Y5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z5">
         <v>1</v>
@@ -3172,10 +3175,10 @@
       </c>
       <c r="X8" s="22"/>
       <c r="Y8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA8">
         <v>30</v>
@@ -3625,7 +3628,7 @@
       </c>
       <c r="X13" s="22"/>
       <c r="Y13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z13">
         <v>1</v>
@@ -3966,10 +3969,10 @@
         <v>36</v>
       </c>
       <c r="O17" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P17" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="23">
         <v>1</v>
@@ -3994,7 +3997,7 @@
       </c>
       <c r="X17" s="22"/>
       <c r="Y17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z17">
         <v>1</v>
@@ -4545,7 +4548,7 @@
       </c>
       <c r="X23" s="22"/>
       <c r="Y23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z23">
         <v>1</v>
@@ -4609,10 +4612,10 @@
         <v>36</v>
       </c>
       <c r="O24" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P24" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q24" s="23">
         <v>1</v>
@@ -5241,25 +5244,22 @@
         <v>24</v>
       </c>
       <c r="K31" s="37">
-        <f t="array" ref="K31">INDEX(Sheet2!$H$2:$I$21,MATCH(G31,Sheet2!$I$2:I49,0),1)</f>
-        <v>27</v>
-      </c>
-      <c r="L31" s="38" t="str">
-        <f t="array" ref="L31">INDEX(Sheet2!$B$2:$C$21,MATCH(G31,Sheet2!$C$2:C64,0),1)</f>
-        <v>sdr</v>
-      </c>
-      <c r="M31" s="39" t="str">
-        <f t="array" ref="M31">INDEX(Sheet2!$E$2:$F$21,MATCH(G31,Sheet2!$F$2:F64,0),1)</f>
-        <v>.gz</v>
+        <v>33</v>
+      </c>
+      <c r="L31" s="38" t="s">
+        <v>202</v>
+      </c>
+      <c r="M31" s="39" t="s">
+        <v>203</v>
       </c>
       <c r="N31" s="22" t="s">
         <v>36</v>
       </c>
       <c r="O31" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P31" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q31" s="23">
         <v>0</v>
@@ -5268,10 +5268,10 @@
         <v>1</v>
       </c>
       <c r="S31" s="22" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="T31" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U31" s="23">
         <v>0</v>
@@ -5284,7 +5284,7 @@
       </c>
       <c r="X31" s="22"/>
       <c r="Y31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z31">
         <v>1</v>
@@ -5316,19 +5316,19 @@
         <v>38</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="F32" s="22" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="G32" s="24" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H32" s="22" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="I32" s="22" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="J32" s="23">
         <v>24</v>
@@ -5347,10 +5347,10 @@
         <v>36</v>
       </c>
       <c r="O32" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P32" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q32" s="23">
         <v>1</v>
@@ -5359,7 +5359,7 @@
         <v>1</v>
       </c>
       <c r="S32" s="22" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="T32" s="23">
         <v>0</v>
@@ -5375,7 +5375,7 @@
       </c>
       <c r="X32" s="22"/>
       <c r="Y32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z32">
         <v>1</v>
@@ -5395,7 +5395,7 @@
     </row>
     <row r="33" s="19" customFormat="1" ht="15" spans="1:30">
       <c r="A33" s="19" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B33" s="35">
         <v>23</v>
@@ -5407,19 +5407,19 @@
         <v>4</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F33" s="19" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="G33" s="19" t="s">
         <v>32</v>
       </c>
       <c r="H33" s="19" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="I33" s="19" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="J33" s="35">
         <v>23</v>
@@ -5427,9 +5427,8 @@
       <c r="K33" s="35">
         <v>29</v>
       </c>
-      <c r="L33" s="47" t="str">
-        <f t="array" ref="L33">INDEX(Sheet2!$B$2:$C$21,MATCH(G33,Sheet2!$C$2:C62,0),1)</f>
-        <v>cdr</v>
+      <c r="L33" s="38" t="s">
+        <v>35</v>
       </c>
       <c r="M33" s="48" t="str">
         <f t="array" ref="M33">INDEX(Sheet2!$E$2:$F$21,MATCH(G33,Sheet2!$F$2:F62,0),1)</f>
@@ -5451,7 +5450,7 @@
         <v>1</v>
       </c>
       <c r="S33" s="19" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="T33" s="35">
         <v>0</v>
@@ -5460,14 +5459,14 @@
         <v>0</v>
       </c>
       <c r="V33" s="19" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="W33">
         <v>314</v>
       </c>
       <c r="X33" s="22"/>
       <c r="Y33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z33">
         <v>1</v>
@@ -5487,7 +5486,7 @@
     </row>
     <row r="34" ht="15" spans="1:30">
       <c r="A34" s="22" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B34" s="23">
         <v>23</v>
@@ -5499,19 +5498,19 @@
         <v>38</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F34" s="22" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G34" s="24" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H34" s="22" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="I34" s="22" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="J34" s="23">
         <v>23</v>
@@ -5530,10 +5529,10 @@
         <v>36</v>
       </c>
       <c r="O34" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P34" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q34" s="23">
         <v>1</v>
@@ -5542,7 +5541,7 @@
         <v>1</v>
       </c>
       <c r="S34" s="22" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="T34" s="23">
         <v>0</v>
@@ -5551,7 +5550,7 @@
         <v>0</v>
       </c>
       <c r="V34" s="22" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="W34">
         <v>315</v>
@@ -5578,7 +5577,7 @@
     </row>
     <row r="35" ht="15" spans="1:30">
       <c r="A35" s="22" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B35" s="23">
         <v>15</v>
@@ -5590,19 +5589,19 @@
         <v>4</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="F35" s="22" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="G35" s="24" t="s">
         <v>49</v>
       </c>
       <c r="H35" s="22" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="I35" s="22" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="J35" s="23">
         <v>15</v>
@@ -5635,7 +5634,7 @@
         <v>1</v>
       </c>
       <c r="S35" s="22" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="T35" s="23">
         <v>0</v>
@@ -5644,7 +5643,7 @@
         <v>0</v>
       </c>
       <c r="V35" s="22" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="W35">
         <v>316</v>
@@ -5671,7 +5670,7 @@
     </row>
     <row r="36" ht="15" spans="1:30">
       <c r="A36" s="22" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B36" s="23">
         <v>15</v>
@@ -5683,19 +5682,19 @@
         <v>38</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="F36" s="22" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G36" s="24" t="s">
         <v>68</v>
       </c>
       <c r="H36" s="22" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="I36" s="22" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="J36" s="23">
         <v>15</v>
@@ -5705,7 +5704,7 @@
         <v>3</v>
       </c>
       <c r="L36" s="38" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="M36" s="39" t="str">
         <f t="array" ref="M36">INDEX(Sheet2!$E$2:$F$21,MATCH(G36,Sheet2!$F$2:F45,0),1)</f>
@@ -5736,7 +5735,7 @@
         <v>0</v>
       </c>
       <c r="V36" s="22" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="W36">
         <v>317</v>
@@ -5763,7 +5762,7 @@
     </row>
     <row r="37" ht="15" spans="1:30">
       <c r="A37" s="22" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B37" s="23">
         <v>16</v>
@@ -5775,19 +5774,19 @@
         <v>4</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="F37" s="22" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G37" s="24" t="s">
         <v>49</v>
       </c>
       <c r="H37" s="22" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="I37" s="22" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="J37" s="23">
         <v>16</v>
@@ -5828,7 +5827,7 @@
         <v>0</v>
       </c>
       <c r="V37" s="22" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="W37">
         <v>318</v>
@@ -5855,7 +5854,7 @@
     </row>
     <row r="38" ht="15" spans="1:30">
       <c r="A38" s="22" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B38" s="23">
         <v>16</v>
@@ -5867,19 +5866,19 @@
         <v>38</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="F38" s="22" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="G38" s="24" t="s">
         <v>68</v>
       </c>
       <c r="H38" s="22" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="I38" s="22" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="J38" s="23">
         <v>16</v>
@@ -5889,7 +5888,7 @@
         <v>3</v>
       </c>
       <c r="L38" s="38" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="M38" s="39" t="str">
         <f t="array" ref="M38">INDEX([1]Sheet2!$E$2:$F$21,MATCH(G38,[1]Sheet2!$F$2:F47,0),1)</f>
@@ -5911,7 +5910,7 @@
         <v>1</v>
       </c>
       <c r="S38" s="22" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="T38" s="23">
         <v>0</v>
@@ -5920,7 +5919,7 @@
         <v>0</v>
       </c>
       <c r="V38" s="22" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="W38">
         <v>319</v>
@@ -5947,7 +5946,7 @@
     </row>
     <row r="39" ht="15" spans="1:30">
       <c r="A39" s="22" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B39" s="23">
         <v>17</v>
@@ -5959,19 +5958,19 @@
         <v>4</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="F39" s="22" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="G39" s="24" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="H39" s="22" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="I39" s="22" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="J39" s="23">
         <v>17</v>
@@ -5983,7 +5982,7 @@
         <v>0</v>
       </c>
       <c r="M39" s="39" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="N39" s="22" t="s">
         <v>36</v>
@@ -6001,7 +6000,7 @@
         <v>1</v>
       </c>
       <c r="S39" s="22" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="T39" s="23">
         <v>0</v>
@@ -6010,14 +6009,14 @@
         <v>0</v>
       </c>
       <c r="V39" s="22" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="W39">
         <v>320</v>
       </c>
       <c r="X39" s="22"/>
       <c r="Y39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z39">
         <v>1</v>
@@ -6037,7 +6036,7 @@
     </row>
     <row r="40" ht="15" spans="1:30">
       <c r="A40" s="22" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B40" s="23">
         <v>17</v>
@@ -6049,19 +6048,19 @@
         <v>38</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F40" s="22" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="G40" s="24" t="s">
         <v>161</v>
       </c>
       <c r="H40" s="22" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="I40" s="22" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="J40" s="23">
         <v>17</v>
@@ -6071,7 +6070,7 @@
         <v>17</v>
       </c>
       <c r="L40" s="38" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="M40" s="39" t="str">
         <f>INDEX(Sheet2!$E$2:$F$21,MATCH(G40,Sheet2!$F$2:F49,0),1)</f>
@@ -6093,7 +6092,7 @@
         <v>1</v>
       </c>
       <c r="S40" s="22" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="T40" s="23">
         <v>0</v>
@@ -6102,7 +6101,7 @@
         <v>0</v>
       </c>
       <c r="V40" s="22" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="W40">
         <v>321</v>
@@ -6129,7 +6128,7 @@
     </row>
     <row r="41" ht="15" spans="1:30">
       <c r="A41" s="22" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B41" s="23">
         <v>20</v>
@@ -6141,19 +6140,19 @@
         <v>4</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="F41" s="22" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="G41" s="24" t="s">
         <v>32</v>
       </c>
       <c r="H41" s="22" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="I41" s="22" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="J41" s="23">
         <v>20</v>
@@ -6186,7 +6185,7 @@
         <v>1</v>
       </c>
       <c r="S41" s="22" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="T41" s="23">
         <v>0</v>
@@ -6195,7 +6194,7 @@
         <v>0</v>
       </c>
       <c r="V41" s="22" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="W41">
         <v>322</v>
@@ -6222,7 +6221,7 @@
     </row>
     <row r="42" ht="15" spans="1:30">
       <c r="A42" s="22" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B42" s="23">
         <v>20</v>
@@ -6234,19 +6233,19 @@
         <v>38</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="F42" s="22" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="G42" s="24" t="s">
         <v>68</v>
       </c>
       <c r="H42" s="22" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="I42" s="22" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="J42" s="23">
         <v>20</v>
@@ -6256,7 +6255,7 @@
         <v>3</v>
       </c>
       <c r="L42" s="38" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="M42" s="39" t="str">
         <f t="array" ref="M42">INDEX(Sheet2!$E$2:$F$21,MATCH(G42,Sheet2!$F$2:F56,0),1)</f>
@@ -6287,7 +6286,7 @@
         <v>0</v>
       </c>
       <c r="V42" s="22" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="W42">
         <v>323</v>
@@ -6314,7 +6313,7 @@
     </row>
     <row r="43" ht="15" spans="1:30">
       <c r="A43" s="22" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B43" s="23">
         <v>21</v>
@@ -6326,19 +6325,19 @@
         <v>4</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="F43" s="22" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="G43" s="24" t="s">
         <v>49</v>
       </c>
       <c r="H43" s="22" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="I43" s="22" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="J43" s="23">
         <v>21</v>
@@ -6379,17 +6378,17 @@
         <v>0</v>
       </c>
       <c r="V43" s="22" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="W43">
         <v>324</v>
       </c>
       <c r="X43" s="22"/>
       <c r="Y43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA43">
         <v>30</v>
@@ -6398,7 +6397,7 @@
         <v>70000</v>
       </c>
       <c r="AC43">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="AD43">
         <v>5</v>
@@ -6406,7 +6405,7 @@
     </row>
     <row r="44" ht="15" spans="1:30">
       <c r="A44" s="22" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B44" s="23">
         <v>21</v>
@@ -6418,19 +6417,19 @@
         <v>38</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="F44" s="22" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="G44" s="24" t="s">
         <v>68</v>
       </c>
       <c r="H44" s="22" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="I44" s="22" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="J44" s="23">
         <v>21</v>
@@ -6472,7 +6471,7 @@
         <v>0</v>
       </c>
       <c r="V44" s="22" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="W44">
         <v>325</v>
@@ -6499,7 +6498,7 @@
     </row>
     <row r="45" ht="15" spans="1:30">
       <c r="A45" s="22" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B45" s="23">
         <v>19</v>
@@ -6511,19 +6510,19 @@
         <v>4</v>
       </c>
       <c r="E45" s="22" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="F45" s="22" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="G45" s="24" t="s">
         <v>49</v>
       </c>
       <c r="H45" s="22" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="I45" s="22" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="J45" s="23">
         <v>19</v>
@@ -6565,7 +6564,7 @@
         <v>0</v>
       </c>
       <c r="V45" s="22" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="W45">
         <v>326</v>
@@ -6592,7 +6591,7 @@
     </row>
     <row r="46" ht="15" spans="1:30">
       <c r="A46" s="22" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B46" s="23">
         <v>19</v>
@@ -6604,19 +6603,19 @@
         <v>38</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="F46" s="22" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="G46" s="24" t="s">
         <v>68</v>
       </c>
       <c r="H46" s="22" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="I46" s="22" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="J46" s="23">
         <v>19</v>
@@ -6626,7 +6625,7 @@
         <v>3</v>
       </c>
       <c r="L46" s="38" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="M46" s="39" t="str">
         <f t="array" ref="M46">INDEX(Sheet2!$E$2:$F$21,MATCH(G46,Sheet2!$F$2:F54,0),1)</f>
@@ -6648,7 +6647,7 @@
         <v>1</v>
       </c>
       <c r="S46" s="22" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="T46" s="23">
         <v>0</v>
@@ -6657,7 +6656,7 @@
         <v>0</v>
       </c>
       <c r="V46" s="22" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="W46">
         <v>327</v>
@@ -6684,7 +6683,7 @@
     </row>
     <row r="47" ht="15" spans="1:30">
       <c r="A47" s="22" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B47" s="23">
         <v>26</v>
@@ -6696,19 +6695,19 @@
         <v>4</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="F47" s="22" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="G47" s="24" t="s">
         <v>62</v>
       </c>
       <c r="H47" s="22" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="I47" s="22" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="J47" s="23">
         <v>26</v>
@@ -6750,7 +6749,7 @@
         <v>0</v>
       </c>
       <c r="V47" s="22" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="W47">
         <v>328</v>
@@ -6777,7 +6776,7 @@
     </row>
     <row r="48" ht="15" spans="1:30">
       <c r="A48" s="22" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B48" s="23">
         <v>26</v>
@@ -6789,19 +6788,19 @@
         <v>38</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="F48" s="22" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="G48" s="24" t="s">
         <v>161</v>
       </c>
       <c r="H48" s="22" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="I48" s="22" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="J48" s="23">
         <v>26</v>
@@ -6834,7 +6833,7 @@
         <v>1</v>
       </c>
       <c r="S48" s="22" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="T48" s="23">
         <v>0</v>
@@ -6843,7 +6842,7 @@
         <v>0</v>
       </c>
       <c r="V48" s="22" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="W48">
         <v>329</v>
@@ -6870,7 +6869,7 @@
     </row>
     <row r="49" s="15" customFormat="1" ht="15" spans="1:30">
       <c r="A49" s="15" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B49" s="25">
         <v>22</v>
@@ -6882,19 +6881,19 @@
         <v>4</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="G49" s="15" t="s">
         <v>49</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="I49" s="15" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="J49" s="25">
         <v>22</v>
@@ -6935,14 +6934,14 @@
         <v>0</v>
       </c>
       <c r="V49" s="15" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="W49">
         <v>330</v>
       </c>
       <c r="X49" s="22"/>
       <c r="Y49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z49">
         <v>1</v>
@@ -6962,7 +6961,7 @@
     </row>
     <row r="50" ht="15" spans="1:30">
       <c r="A50" s="22" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B50" s="23">
         <v>22</v>
@@ -6974,19 +6973,19 @@
         <v>38</v>
       </c>
       <c r="E50" s="22" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="F50" s="22" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="G50" s="24" t="s">
         <v>68</v>
       </c>
       <c r="H50" s="22" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="I50" s="22" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="J50" s="23">
         <v>22</v>
@@ -7019,7 +7018,7 @@
         <v>1</v>
       </c>
       <c r="S50" s="22" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="T50" s="23">
         <v>0</v>
@@ -7028,7 +7027,7 @@
         <v>1</v>
       </c>
       <c r="V50" s="22" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="W50">
         <v>331</v>
@@ -7055,7 +7054,7 @@
     </row>
     <row r="51" ht="15" spans="1:30">
       <c r="A51" s="22" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B51" s="23">
         <v>22</v>
@@ -7067,19 +7066,19 @@
         <v>38</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="F51" s="22" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="G51" s="33" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="H51" s="22" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="I51" s="22" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="J51" s="23">
         <v>22</v>
@@ -7111,7 +7110,7 @@
         <v>1</v>
       </c>
       <c r="S51" s="22" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="T51" s="23">
         <v>0</v>
@@ -7120,7 +7119,7 @@
         <v>0</v>
       </c>
       <c r="V51" s="22" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="W51">
         <v>332</v>
@@ -7149,7 +7148,7 @@
     </row>
     <row r="52" s="20" customFormat="1" ht="15" spans="1:30">
       <c r="A52" s="20" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B52" s="36">
         <v>25</v>
@@ -7161,19 +7160,19 @@
         <v>4</v>
       </c>
       <c r="E52" s="20" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="F52" s="20" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="G52" s="20" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="H52" s="20" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="I52" s="20" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="J52" s="36">
         <v>25</v>
@@ -7201,7 +7200,7 @@
         <v>1</v>
       </c>
       <c r="S52" s="20" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="T52" s="36">
         <v>0</v>
@@ -7210,14 +7209,14 @@
         <v>0</v>
       </c>
       <c r="V52" s="20" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="W52">
         <v>333</v>
       </c>
       <c r="X52" s="22"/>
       <c r="Y52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z52">
         <v>1</v>
@@ -7237,7 +7236,7 @@
     </row>
     <row r="53" ht="15" spans="1:30">
       <c r="A53" s="22" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B53" s="23">
         <v>25</v>
@@ -7249,19 +7248,19 @@
         <v>38</v>
       </c>
       <c r="E53" s="22" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="F53" s="22" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="G53" s="24" t="s">
         <v>68</v>
       </c>
       <c r="H53" s="22" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="I53" s="22" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="J53" s="23">
         <v>25</v>
@@ -7281,10 +7280,10 @@
         <v>36</v>
       </c>
       <c r="O53" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P53" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q53" s="23">
         <v>1</v>
@@ -7293,7 +7292,7 @@
         <v>1</v>
       </c>
       <c r="S53" s="22" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="T53" s="23">
         <v>0</v>
@@ -7302,7 +7301,7 @@
         <v>0</v>
       </c>
       <c r="V53" s="22" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="W53">
         <v>334</v>
@@ -7329,7 +7328,7 @@
     </row>
     <row r="54" ht="15" spans="1:30">
       <c r="A54" s="22" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B54" s="23">
         <v>27</v>
@@ -7341,19 +7340,19 @@
         <v>4</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="F54" s="22" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="G54" s="24" t="s">
         <v>32</v>
       </c>
       <c r="H54" s="22" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="I54" s="22" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="J54" s="23">
         <v>27</v>
@@ -7384,7 +7383,7 @@
         <v>1</v>
       </c>
       <c r="S54" s="22" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="T54" s="23">
         <v>0</v>
@@ -7393,14 +7392,14 @@
         <v>0</v>
       </c>
       <c r="V54" s="22" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="W54">
         <v>335</v>
       </c>
       <c r="X54" s="22"/>
       <c r="Y54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z54">
         <v>1</v>
@@ -7420,7 +7419,7 @@
     </row>
     <row r="55" ht="15" spans="1:30">
       <c r="A55" s="22" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B55" s="23">
         <v>27</v>
@@ -7432,19 +7431,19 @@
         <v>38</v>
       </c>
       <c r="E55" s="22" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="F55" s="22" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="G55" s="24" t="s">
         <v>68</v>
       </c>
       <c r="H55" s="22" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="I55" s="22" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="J55" s="23">
         <v>27</v>
@@ -7476,7 +7475,7 @@
         <v>0</v>
       </c>
       <c r="S55" s="22" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="T55" s="23">
         <v>0</v>
@@ -7485,7 +7484,7 @@
         <v>0</v>
       </c>
       <c r="V55" s="22" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="W55">
         <v>336</v>
@@ -7539,24 +7538,24 @@
     <row r="1" ht="12.75" customHeight="1" spans="1:26">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="2" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>337</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>335</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -7578,14 +7577,14 @@
     </row>
     <row r="2" ht="12.75" customHeight="1" spans="2:9">
       <c r="B2" s="6" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>68</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="6" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>68</v>
@@ -7600,14 +7599,14 @@
     </row>
     <row r="3" ht="12.75" customHeight="1" spans="2:9">
       <c r="B3" s="6" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="6" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>41</v>
@@ -7622,14 +7621,14 @@
     </row>
     <row r="4" ht="12.75" customHeight="1" spans="2:9">
       <c r="B4" s="6" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>49</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="6" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>49</v>
@@ -7644,14 +7643,14 @@
     </row>
     <row r="5" ht="12.75" customHeight="1" spans="2:9">
       <c r="B5" s="6" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>161</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="6" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>161</v>
@@ -7666,14 +7665,14 @@
     </row>
     <row r="6" ht="12.75" customHeight="1" spans="2:9">
       <c r="B6" s="6" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="6" t="s">
-        <v>346</v>
+        <v>203</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>32</v>
@@ -7688,36 +7687,36 @@
     </row>
     <row r="7" ht="12.75" customHeight="1" spans="2:9">
       <c r="B7" s="9" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="6" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="9">
         <v>36</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1" spans="2:9">
       <c r="B8" s="6" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>62</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="6" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>62</v>
@@ -7732,24 +7731,24 @@
     </row>
     <row r="9" ht="12.75" customHeight="1" spans="2:9">
       <c r="B9" s="11" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="13" t="s">
         <v>116</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="11">
         <v>37</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1" spans="2:9">
@@ -7757,41 +7756,41 @@
         <v>2</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="11">
         <v>38</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1" spans="2:9">
       <c r="B11" s="11" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="11" t="s">
-        <v>346</v>
+        <v>203</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="11">
         <v>39</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1" spans="2:9">
@@ -7899,7 +7898,7 @@
     <row r="24" ht="12.75" customHeight="1"/>
     <row r="25" ht="12.75" customHeight="1" spans="3:3">
       <c r="C25" s="14" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="26" ht="12.75" customHeight="1"/>

</xml_diff>

<commit_message>
Fixed Optimizeer of Gazi
</commit_message>
<xml_diff>
--- a/TelcobrightVS13/Projects/UtilInstallConfig/config/cas/_helper/casOperatorInfo.xlsx
+++ b/TelcobrightVS13/Projects/UtilInstallConfig/config/cas/_helper/casOperatorInfo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8760"/>
+    <workbookView windowWidth="28800" windowHeight="11880"/>
   </bookViews>
   <sheets>
     <sheet name="NE automation data" sheetId="3" r:id="rId1"/>
@@ -413,7 +413,7 @@
     <t>iRX6IRZsPP8gfnW</t>
   </si>
   <si>
-    <t>d:\telcobright\vault\resources\cdr\gaziNetworks\tdm</t>
+    <t>U:\telcobright\vault\resources\cdr\gaziNetworks\tdm</t>
   </si>
   <si>
     <t>GAZI</t>
@@ -431,7 +431,7 @@
     <t>RitUtipi9Ras25je</t>
   </si>
   <si>
-    <t>D:\telcobright\vault\resources\CDR\gazinetworks\tdmKhlBogra\Khulna</t>
+    <t>U:\telcobright\vault\resources\CDR\gazinetworks\tdmKhlBogra\Khulna</t>
   </si>
   <si>
     <t>GNL</t>
@@ -443,7 +443,7 @@
     <t>TELCOBRIDGE_BOGRA</t>
   </si>
   <si>
-    <t>D:\telcobright\vault\resources\CDR\gazinetworks\tdmKhlBogra\bogra</t>
+    <t>U:\telcobright\vault\resources\CDR\gazinetworks\tdmKhlBogra\bogra</t>
   </si>
   <si>
     <t>Vault.TelcobridgeBogra</t>
@@ -2424,10 +2424,10 @@
   <sheetPr/>
   <dimension ref="A1:AD55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="AF29" sqref="AF29"/>
+      <selection pane="bottomLeft" activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -2783,10 +2783,10 @@
         <v>36</v>
       </c>
       <c r="O4" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="23">
         <v>1</v>
@@ -2871,10 +2871,10 @@
         <v>36</v>
       </c>
       <c r="O5" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5" s="23">
         <v>1</v>

</xml_diff>